<commit_message>
Update slicing participant de6bec443fc3a55b95d2844759ea3542f5545502
</commit_message>
<xml_diff>
--- a/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-encounter-evenement.xlsx
+++ b/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-encounter-evenement.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-30T16:47:22+00:00</t>
+    <t>2025-10-01T14:45:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1867,9 +1867,6 @@
     <t>http://hl7.org/fhir/ValueSet/encounter-participant-type|4.0.1</t>
   </si>
   <si>
-    <t>Statut.auteur</t>
-  </si>
-  <si>
     <t>Event.performer.function</t>
   </si>
   <si>
@@ -1907,81 +1904,85 @@
     <t>Persons involved in the encounter other than the patient.</t>
   </si>
   <si>
+    <t>Event.performer.actor</t>
+  </si>
+  <si>
+    <t>.role</t>
+  </si>
+  <si>
+    <t>FiveWs.who</t>
+  </si>
+  <si>
+    <t>ROL-4</t>
+  </si>
+  <si>
+    <t>Encounter.participant:auteurStatut</t>
+  </si>
+  <si>
+    <t>auteurStatut</t>
+  </si>
+  <si>
+    <t>Professionnel ayant effectué la dernière modification du statut associé à la ressource.</t>
+  </si>
+  <si>
+    <t>Statut.auteur</t>
+  </si>
+  <si>
+    <t>Encounter.participant:auteurStatut.id</t>
+  </si>
+  <si>
+    <t>Encounter.participant:auteurStatut.extension</t>
+  </si>
+  <si>
+    <t>Encounter.participant:auteurStatut.modifierExtension</t>
+  </si>
+  <si>
+    <t>Encounter.participant:auteurStatut.type</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="https://interop.esante.gouv.fr/ig/fhir/tddui/CodeSystem/TDDUIEncounterParticipant"/&gt;
+    &lt;code value="AUT"/&gt;
+    &lt;display value="Auteur du statut de la ressource"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
+  </si>
+  <si>
+    <t>Encounter.participant:auteurStatut.period</t>
+  </si>
+  <si>
+    <t>Encounter.participant:auteurStatut.individual</t>
+  </si>
+  <si>
+    <t>Encounter.participant:professionnel</t>
+  </si>
+  <si>
+    <t>professionnel</t>
+  </si>
+  <si>
+    <t>List of participants involved in the encounter</t>
+  </si>
+  <si>
     <t>Professionnel</t>
   </si>
   <si>
-    <t>Event.performer.actor</t>
-  </si>
-  <si>
-    <t>.role</t>
-  </si>
-  <si>
-    <t>FiveWs.who</t>
-  </si>
-  <si>
-    <t>ROL-4</t>
-  </si>
-  <si>
-    <t>Encounter.participant:auteurStatut</t>
-  </si>
-  <si>
-    <t>auteurStatut</t>
-  </si>
-  <si>
-    <t>Professionnel ayant effectué la dernière modification du statut associé à la ressource.</t>
-  </si>
-  <si>
-    <t>Encounter.participant:auteurStatut.id</t>
-  </si>
-  <si>
-    <t>Encounter.participant:auteurStatut.extension</t>
-  </si>
-  <si>
-    <t>Encounter.participant:auteurStatut.modifierExtension</t>
-  </si>
-  <si>
-    <t>Encounter.participant:auteurStatut.type</t>
+    <t>Encounter.participant:professionnel.id</t>
+  </si>
+  <si>
+    <t>Encounter.participant:professionnel.extension</t>
+  </si>
+  <si>
+    <t>Encounter.participant:professionnel.modifierExtension</t>
+  </si>
+  <si>
+    <t>Encounter.participant:professionnel.type</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
     &lt;system value="http://terminology.hl7.org/CodeSystem/v3-ParticipationType"/&gt;
     &lt;code value="PART"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t>Encounter.participant:auteurStatut.period</t>
-  </si>
-  <si>
-    <t>Encounter.participant:auteurStatut.individual</t>
-  </si>
-  <si>
-    <t>Encounter.participant:professionnel</t>
-  </si>
-  <si>
-    <t>professionnel</t>
-  </si>
-  <si>
-    <t>List of participants involved in the encounter</t>
-  </si>
-  <si>
-    <t>Encounter.participant:professionnel.id</t>
-  </si>
-  <si>
-    <t>Encounter.participant:professionnel.extension</t>
-  </si>
-  <si>
-    <t>Encounter.participant:professionnel.modifierExtension</t>
-  </si>
-  <si>
-    <t>Encounter.participant:professionnel.type</t>
-  </si>
-  <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="http://terminology.hl7.org/CodeSystem/v3-ParticipationType"/&gt;
-    &lt;code value="PPRF"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
@@ -17902,27 +17903,27 @@
         <v>103</v>
       </c>
       <c r="AK128" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL128" t="s" s="2">
         <v>599</v>
       </c>
-      <c r="AL128" t="s" s="2">
+      <c r="AM128" t="s" s="2">
         <v>600</v>
       </c>
-      <c r="AM128" t="s" s="2">
+      <c r="AN128" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AO128" t="s" s="2">
         <v>601</v>
-      </c>
-      <c r="AN128" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AO128" t="s" s="2">
-        <v>602</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" t="s" s="2">
@@ -17948,10 +17949,10 @@
         <v>345</v>
       </c>
       <c r="L129" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="M129" t="s" s="2">
         <v>604</v>
-      </c>
-      <c r="M129" t="s" s="2">
-        <v>605</v>
       </c>
       <c r="N129" s="2"/>
       <c r="O129" s="2"/>
@@ -18002,7 +18003,7 @@
         <v>82</v>
       </c>
       <c r="AF129" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AG129" t="s" s="2">
         <v>80</v>
@@ -18023,21 +18024,21 @@
         <v>82</v>
       </c>
       <c r="AM129" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="AN129" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AO129" t="s" s="2">
         <v>606</v>
-      </c>
-      <c r="AN129" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AO129" t="s" s="2">
-        <v>607</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" t="s" s="2">
@@ -18060,13 +18061,13 @@
         <v>92</v>
       </c>
       <c r="K130" t="s" s="2">
+        <v>608</v>
+      </c>
+      <c r="L130" t="s" s="2">
         <v>609</v>
       </c>
-      <c r="L130" t="s" s="2">
+      <c r="M130" t="s" s="2">
         <v>610</v>
-      </c>
-      <c r="M130" t="s" s="2">
-        <v>611</v>
       </c>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
@@ -18117,7 +18118,7 @@
         <v>82</v>
       </c>
       <c r="AF130" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AG130" t="s" s="2">
         <v>80</v>
@@ -18132,30 +18133,30 @@
         <v>103</v>
       </c>
       <c r="AK130" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL130" t="s" s="2">
+        <v>611</v>
+      </c>
+      <c r="AM130" t="s" s="2">
         <v>612</v>
       </c>
-      <c r="AL130" t="s" s="2">
+      <c r="AN130" t="s" s="2">
         <v>613</v>
       </c>
-      <c r="AM130" t="s" s="2">
+      <c r="AO130" t="s" s="2">
         <v>614</v>
-      </c>
-      <c r="AN130" t="s" s="2">
-        <v>615</v>
-      </c>
-      <c r="AO130" t="s" s="2">
-        <v>616</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s" s="2">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B131" t="s" s="2">
         <v>584</v>
       </c>
       <c r="C131" t="s" s="2">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D131" t="s" s="2">
         <v>82</v>
@@ -18180,7 +18181,7 @@
         <v>384</v>
       </c>
       <c r="L131" t="s" s="2">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="M131" t="s" s="2">
         <v>586</v>
@@ -18249,7 +18250,7 @@
         <v>103</v>
       </c>
       <c r="AK131" t="s" s="2">
-        <v>82</v>
+        <v>618</v>
       </c>
       <c r="AL131" t="s" s="2">
         <v>588</v>
@@ -18266,7 +18267,7 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="2">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B132" t="s" s="2">
         <v>591</v>
@@ -18381,7 +18382,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B133" t="s" s="2">
         <v>592</v>
@@ -18498,7 +18499,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B134" t="s" s="2">
         <v>593</v>
@@ -18617,7 +18618,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B135" t="s" s="2">
         <v>594</v>
@@ -18663,7 +18664,7 @@
         <v>82</v>
       </c>
       <c r="S135" t="s" s="2">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T135" t="s" s="2">
         <v>82</v>
@@ -18720,24 +18721,24 @@
         <v>82</v>
       </c>
       <c r="AL135" t="s" s="2">
+        <v>599</v>
+      </c>
+      <c r="AM135" t="s" s="2">
         <v>600</v>
       </c>
-      <c r="AM135" t="s" s="2">
+      <c r="AN135" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AO135" t="s" s="2">
         <v>601</v>
-      </c>
-      <c r="AN135" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AO135" t="s" s="2">
-        <v>602</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B136" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" t="s" s="2">
@@ -18763,10 +18764,10 @@
         <v>345</v>
       </c>
       <c r="L136" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="M136" t="s" s="2">
         <v>604</v>
-      </c>
-      <c r="M136" t="s" s="2">
-        <v>605</v>
       </c>
       <c r="N136" s="2"/>
       <c r="O136" s="2"/>
@@ -18817,7 +18818,7 @@
         <v>82</v>
       </c>
       <c r="AF136" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AG136" t="s" s="2">
         <v>80</v>
@@ -18838,21 +18839,21 @@
         <v>82</v>
       </c>
       <c r="AM136" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="AN136" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AO136" t="s" s="2">
         <v>606</v>
-      </c>
-      <c r="AN136" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AO136" t="s" s="2">
-        <v>607</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s" s="2">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B137" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C137" s="2"/>
       <c r="D137" t="s" s="2">
@@ -18875,13 +18876,13 @@
         <v>92</v>
       </c>
       <c r="K137" t="s" s="2">
+        <v>608</v>
+      </c>
+      <c r="L137" t="s" s="2">
         <v>609</v>
       </c>
-      <c r="L137" t="s" s="2">
+      <c r="M137" t="s" s="2">
         <v>610</v>
-      </c>
-      <c r="M137" t="s" s="2">
-        <v>611</v>
       </c>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
@@ -18932,7 +18933,7 @@
         <v>82</v>
       </c>
       <c r="AF137" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AG137" t="s" s="2">
         <v>80</v>
@@ -18950,27 +18951,27 @@
         <v>82</v>
       </c>
       <c r="AL137" t="s" s="2">
+        <v>611</v>
+      </c>
+      <c r="AM137" t="s" s="2">
+        <v>612</v>
+      </c>
+      <c r="AN137" t="s" s="2">
         <v>613</v>
       </c>
-      <c r="AM137" t="s" s="2">
+      <c r="AO137" t="s" s="2">
         <v>614</v>
-      </c>
-      <c r="AN137" t="s" s="2">
-        <v>615</v>
-      </c>
-      <c r="AO137" t="s" s="2">
-        <v>616</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s" s="2">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B138" t="s" s="2">
         <v>584</v>
       </c>
       <c r="C138" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D138" t="s" s="2">
         <v>82</v>
@@ -18995,7 +18996,7 @@
         <v>384</v>
       </c>
       <c r="L138" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="M138" t="s" s="2">
         <v>586</v>
@@ -19064,7 +19065,7 @@
         <v>103</v>
       </c>
       <c r="AK138" t="s" s="2">
-        <v>82</v>
+        <v>629</v>
       </c>
       <c r="AL138" t="s" s="2">
         <v>588</v>
@@ -19535,16 +19536,16 @@
         <v>82</v>
       </c>
       <c r="AL142" t="s" s="2">
+        <v>599</v>
+      </c>
+      <c r="AM142" t="s" s="2">
         <v>600</v>
       </c>
-      <c r="AM142" t="s" s="2">
+      <c r="AN142" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AO142" t="s" s="2">
         <v>601</v>
-      </c>
-      <c r="AN142" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AO142" t="s" s="2">
-        <v>602</v>
       </c>
     </row>
     <row r="143">
@@ -19552,7 +19553,7 @@
         <v>635</v>
       </c>
       <c r="B143" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C143" s="2"/>
       <c r="D143" t="s" s="2">
@@ -19578,10 +19579,10 @@
         <v>345</v>
       </c>
       <c r="L143" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="M143" t="s" s="2">
         <v>604</v>
-      </c>
-      <c r="M143" t="s" s="2">
-        <v>605</v>
       </c>
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
@@ -19632,7 +19633,7 @@
         <v>82</v>
       </c>
       <c r="AF143" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AG143" t="s" s="2">
         <v>80</v>
@@ -19653,13 +19654,13 @@
         <v>82</v>
       </c>
       <c r="AM143" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="AN143" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AO143" t="s" s="2">
         <v>606</v>
-      </c>
-      <c r="AN143" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AO143" t="s" s="2">
-        <v>607</v>
       </c>
     </row>
     <row r="144">
@@ -19667,7 +19668,7 @@
         <v>636</v>
       </c>
       <c r="B144" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144" t="s" s="2">
@@ -19690,13 +19691,13 @@
         <v>92</v>
       </c>
       <c r="K144" t="s" s="2">
+        <v>608</v>
+      </c>
+      <c r="L144" t="s" s="2">
         <v>609</v>
       </c>
-      <c r="L144" t="s" s="2">
+      <c r="M144" t="s" s="2">
         <v>610</v>
-      </c>
-      <c r="M144" t="s" s="2">
-        <v>611</v>
       </c>
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
@@ -19747,7 +19748,7 @@
         <v>82</v>
       </c>
       <c r="AF144" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AG144" t="s" s="2">
         <v>80</v>
@@ -19765,16 +19766,16 @@
         <v>82</v>
       </c>
       <c r="AL144" t="s" s="2">
+        <v>611</v>
+      </c>
+      <c r="AM144" t="s" s="2">
+        <v>612</v>
+      </c>
+      <c r="AN144" t="s" s="2">
         <v>613</v>
       </c>
-      <c r="AM144" t="s" s="2">
+      <c r="AO144" t="s" s="2">
         <v>614</v>
-      </c>
-      <c r="AN144" t="s" s="2">
-        <v>615</v>
-      </c>
-      <c r="AO144" t="s" s="2">
-        <v>616</v>
       </c>
     </row>
     <row r="145">
@@ -24773,7 +24774,7 @@
         <v>812</v>
       </c>
       <c r="AM187" t="s" s="2">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="AN187" t="s" s="2">
         <v>813</v>
@@ -25120,7 +25121,7 @@
         <v>82</v>
       </c>
       <c r="AM190" t="s" s="2">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AN190" t="s" s="2">
         <v>82</v>
@@ -25232,7 +25233,7 @@
         <v>834</v>
       </c>
       <c r="AL191" t="s" s="2">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="AM191" t="s" s="2">
         <v>835</v>

</xml_diff>